<commit_message>
Updated scripts and sources
</commit_message>
<xml_diff>
--- a/00-Phylogenetics/CKI1/01-Input/List_of_OneKP.xlsx
+++ b/00-Phylogenetics/CKI1/01-Input/List_of_OneKP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunrui/Library/CloudStorage/OneDrive-Personal/Marchantia/Manuscripts/202304-MpCKI1/Github_submission/repos/00-Phylogenetics/CKI1/01-Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/312e60aa730c1faf/Marchantia/Manuscripts/202304-MpCKI1/02-Github_submission/repos/00-Phylogenetics/CKI1/01-Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9EA9F0-60D5-A948-9861-EAC213F67209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{1D9EA9F0-60D5-A948-9861-EAC213F67209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F82C6F1-4D4E-5B41-AFC3-A1CCA4B2E67B}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="3820" windowWidth="26840" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="1055">
   <si>
     <t>Code</t>
   </si>
@@ -4032,7 +4032,7 @@
   <dimension ref="A1:E356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D255" sqref="D255"/>
+      <selection activeCell="D234" sqref="D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6914,7 +6914,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>50</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>194</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>781</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>161</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>747</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>191</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>718</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>879</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>890</v>
       </c>
@@ -7067,7 +7067,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>1018</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>40</v>
       </c>
@@ -7101,7 +7101,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>571</v>
       </c>
@@ -7118,7 +7118,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>924</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>20</v>
       </c>
@@ -7152,7 +7152,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>712</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>336</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>756</v>
       </c>
@@ -7203,7 +7203,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>116</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>550</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>750</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>996</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>964</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>976</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>368</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>600</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>428</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>819</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>307</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>92</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>898</v>
       </c>
@@ -7504,11 +7504,8 @@
       <c r="D241" t="s">
         <v>900</v>
       </c>
-      <c r="E241" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>342</v>
       </c>
@@ -7525,7 +7522,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>451</v>
       </c>
@@ -7542,7 +7539,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>286</v>
       </c>
@@ -7947,7 +7944,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>904</v>
       </c>
@@ -7964,7 +7961,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>647</v>
       </c>
@@ -7981,7 +7978,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>1038</v>
       </c>
@@ -7998,7 +7995,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>901</v>
       </c>
@@ -8015,7 +8012,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>386</v>
       </c>
@@ -8032,7 +8029,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>310</v>
       </c>
@@ -8049,7 +8046,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>744</v>
       </c>
@@ -8080,7 +8077,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>837</v>
       </c>
@@ -8097,7 +8094,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>481</v>
       </c>
@@ -8114,7 +8111,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>529</v>
       </c>
@@ -8131,7 +8128,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>56</v>
       </c>
@@ -8148,7 +8145,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>410</v>
       </c>
@@ -8179,7 +8176,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>1005</v>
       </c>
@@ -8196,7 +8193,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>858</v>
       </c>
@@ -8213,7 +8210,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>685</v>
       </c>
@@ -8230,7 +8227,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>1008</v>
       </c>
@@ -8247,7 +8244,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>325</v>
       </c>
@@ -8264,7 +8261,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>915</v>
       </c>
@@ -8281,7 +8278,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>759</v>
       </c>
@@ -8298,7 +8295,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>122</v>
       </c>
@@ -8315,7 +8312,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>586</v>
       </c>
@@ -8346,7 +8343,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>74</v>
       </c>
@@ -8363,7 +8360,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>741</v>
       </c>
@@ -8380,7 +8377,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>644</v>
       </c>
@@ -8397,7 +8394,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>4</v>
       </c>
@@ -8414,7 +8411,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>677</v>
       </c>
@@ -8431,7 +8428,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>362</v>
       </c>
@@ -8448,7 +8445,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>959</v>
       </c>
@@ -8465,7 +8462,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>95</v>
       </c>
@@ -8524,7 +8521,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>460</v>
       </c>
@@ -8555,7 +8552,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>727</v>
       </c>
@@ -8568,11 +8565,8 @@
       <c r="D305" t="s">
         <v>729</v>
       </c>
-      <c r="E305" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>316</v>
       </c>
@@ -8589,7 +8583,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>173</v>
       </c>
@@ -8606,7 +8600,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>1029</v>
       </c>
@@ -8623,7 +8617,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>659</v>
       </c>
@@ -8640,7 +8634,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>149</v>
       </c>
@@ -8685,7 +8679,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>146</v>
       </c>
@@ -8702,7 +8696,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>650</v>
       </c>
@@ -8719,7 +8713,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>861</v>
       </c>
@@ -8736,7 +8730,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>292</v>
       </c>
@@ -8753,7 +8747,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>490</v>
       </c>
@@ -8770,7 +8764,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>295</v>
       </c>
@@ -8787,7 +8781,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>736</v>
       </c>
@@ -8804,7 +8798,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>884</v>
       </c>
@@ -8821,7 +8815,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>77</v>
       </c>
@@ -8838,7 +8832,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>706</v>
       </c>
@@ -8855,7 +8849,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>697</v>
       </c>
@@ -8872,7 +8866,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>994</v>
       </c>
@@ -8889,7 +8883,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>389</v>
       </c>
@@ -8906,7 +8900,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>831</v>
       </c>
@@ -8923,7 +8917,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>137</v>
       </c>
@@ -8940,7 +8934,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>71</v>
       </c>
@@ -8957,7 +8951,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>277</v>
       </c>
@@ -8974,7 +8968,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>413</v>
       </c>
@@ -9075,7 +9069,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>466</v>
       </c>
@@ -9092,7 +9086,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>1035</v>
       </c>
@@ -9109,7 +9103,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>199</v>
       </c>
@@ -9126,7 +9120,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>425</v>
       </c>
@@ -9143,7 +9137,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>244</v>
       </c>
@@ -9188,7 +9182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>700</v>
       </c>
@@ -9205,7 +9199,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>733</v>
       </c>
@@ -9222,7 +9216,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>496</v>
       </c>
@@ -9239,7 +9233,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>953</v>
       </c>
@@ -9256,7 +9250,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>280</v>
       </c>
@@ -9273,7 +9267,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>541</v>
       </c>
@@ -9290,7 +9284,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>765</v>
       </c>
@@ -9307,7 +9301,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>351</v>
       </c>
@@ -9324,7 +9318,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>876</v>
       </c>
@@ -9341,7 +9335,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="353" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>703</v>
       </c>
@@ -9358,7 +9352,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="354" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>235</v>
       </c>
@@ -9389,7 +9383,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="356" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>478</v>
       </c>
@@ -9408,10 +9402,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E356" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Lycophytes"/>
-      </filters>
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A203:E356">
       <sortCondition ref="B1:B356"/>

</xml_diff>